<commit_message>
finish inventory logic (not tested)
</commit_message>
<xml_diff>
--- a/Assets/Info/InventoryConfigInfo/InventoryConfigInfo.xlsx
+++ b/Assets/Info/InventoryConfigInfo/InventoryConfigInfo.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
   <si>
     <t xml:space="preserve">itemId</t>
   </si>
   <si>
     <t xml:space="preserve">maxStackSize</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxStackCount</t>
   </si>
   <si>
     <t xml:space="preserve">key_1</t>
@@ -113,24 +110,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -257,40 +246,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D14" activeCellId="0" sqref="D14"/>
+      <selection pane="topLeft" activeCell="D13" activeCellId="0" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="20.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="20.8"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="27.22"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="11.53"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="2" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" s="2" t="n">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="n">
         <v>1</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>